<commit_message>
feat: add custom basis calculations
</commit_message>
<xml_diff>
--- a/app/data/basisdaten_clean_2025.xlsx
+++ b/app/data/basisdaten_clean_2025.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/guadaluperomero/ProjectsTSB/innovationserhebung/app/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1FE18450-3EEE-3D44-B7E2-EA5A6101D50D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3BDCC98A-641E-2A41-AC3E-CF77B3DF2AA4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-10900" yWindow="-28300" windowWidth="26620" windowHeight="26520" xr2:uid="{25BCFA3D-CBEA-9B42-8B95-A0D09F81B565}"/>
+    <workbookView xWindow="-10860" yWindow="-28300" windowWidth="26620" windowHeight="26520" activeTab="1" xr2:uid="{25BCFA3D-CBEA-9B42-8B95-A0D09F81B565}"/>
   </bookViews>
   <sheets>
     <sheet name="basis_2012_ber" sheetId="63" r:id="rId1"/>
@@ -91,7 +91,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3949" uniqueCount="134">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3951" uniqueCount="134">
   <si>
     <t>Nr. der Klas-
 sifikation</t>
@@ -716,7 +716,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="112">
+  <cellXfs count="113">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -959,6 +959,7 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="1" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1418,15 +1419,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DD24EB00-001C-EA4B-9BA6-7E5E29920E2C}">
-  <dimension ref="A1:H38"/>
+  <dimension ref="A1:I38"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="125" workbookViewId="0">
-      <selection activeCell="G10" sqref="G10"/>
+    <sheetView zoomScale="125" workbookViewId="0">
+      <selection activeCell="I39" sqref="I39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:8" ht="48" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9" ht="48" x14ac:dyDescent="0.2">
       <c r="A1" s="13" t="s">
         <v>133</v>
       </c>
@@ -1451,8 +1452,11 @@
       <c r="H1" s="3" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I1" s="16" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2" s="6" t="s">
         <v>8</v>
       </c>
@@ -1477,8 +1481,11 @@
       <c r="H2" s="8">
         <v>16</v>
       </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I2" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A3" s="6" t="s">
         <v>10</v>
       </c>
@@ -1503,8 +1510,11 @@
       <c r="H3" s="8">
         <v>531</v>
       </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I3" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A4" s="6" t="s">
         <v>12</v>
       </c>
@@ -1529,8 +1539,11 @@
       <c r="H4" s="8">
         <v>1</v>
       </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I4" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A5" s="6" t="s">
         <v>14</v>
       </c>
@@ -1555,8 +1568,11 @@
       <c r="H5" s="8">
         <v>5</v>
       </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I5" s="112">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A6" s="6" t="s">
         <v>16</v>
       </c>
@@ -1581,8 +1597,11 @@
       <c r="H6" s="8">
         <v>520</v>
       </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I6" s="112">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A7" s="6" t="s">
         <v>18</v>
       </c>
@@ -1607,8 +1626,11 @@
       <c r="H7" s="8">
         <v>241</v>
       </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I7" s="112">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A8" s="6" t="s">
         <v>20</v>
       </c>
@@ -1633,8 +1655,11 @@
       <c r="H8" s="8">
         <v>19</v>
       </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I8" s="112">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A9" s="6" t="s">
         <v>22</v>
       </c>
@@ -1659,8 +1684,11 @@
       <c r="H9" s="8">
         <v>12</v>
       </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I9" s="112">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A10" s="6" t="s">
         <v>24</v>
       </c>
@@ -1685,8 +1713,11 @@
       <c r="H10" s="8">
         <v>26</v>
       </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I10" s="112">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A11" s="6" t="s">
         <v>26</v>
       </c>
@@ -1711,8 +1742,11 @@
       <c r="H11" s="8">
         <v>124</v>
       </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I11" s="112">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A12" s="6" t="s">
         <v>28</v>
       </c>
@@ -1737,8 +1771,11 @@
       <c r="H12" s="8">
         <v>37</v>
       </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I12" s="112">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A13" s="6" t="s">
         <v>30</v>
       </c>
@@ -1763,8 +1800,11 @@
       <c r="H13" s="8">
         <v>18</v>
       </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I13" s="112">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A14" s="6" t="s">
         <v>32</v>
       </c>
@@ -1789,8 +1829,11 @@
       <c r="H14" s="8">
         <v>16</v>
       </c>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I14" s="112">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A15" s="6" t="s">
         <v>34</v>
       </c>
@@ -1815,8 +1858,11 @@
       <c r="H15" s="8">
         <v>120</v>
       </c>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I15" s="112">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A16" s="6" t="s">
         <v>36</v>
       </c>
@@ -1841,8 +1887,11 @@
       <c r="H16" s="8">
         <v>26</v>
       </c>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I16" s="112">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A17" s="6"/>
       <c r="B17" s="1"/>
       <c r="C17" s="5"/>
@@ -1852,7 +1901,7 @@
       <c r="G17" s="1"/>
       <c r="H17" s="1"/>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A18" s="6" t="s">
         <v>38</v>
       </c>
@@ -1877,8 +1926,11 @@
       <c r="H18" s="8">
         <v>1345</v>
       </c>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I18" s="112">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A19" s="6" t="s">
         <v>40</v>
       </c>
@@ -1903,8 +1955,11 @@
       <c r="H19" s="8">
         <v>367</v>
       </c>
-    </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I19" s="112">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A20" s="6"/>
       <c r="B20" s="1"/>
       <c r="C20" s="7"/>
@@ -1914,7 +1969,7 @@
       <c r="G20" s="8"/>
       <c r="H20" s="8"/>
     </row>
-    <row r="21" spans="1:8" ht="24" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:9" ht="24" x14ac:dyDescent="0.2">
       <c r="A21" s="9" t="s">
         <v>42</v>
       </c>
@@ -1939,8 +1994,11 @@
       <c r="H21" s="11">
         <v>1713</v>
       </c>
-    </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I21" s="112">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A22" s="6"/>
       <c r="B22" s="1"/>
       <c r="C22" s="5"/>
@@ -1950,7 +2008,7 @@
       <c r="G22" s="1"/>
       <c r="H22" s="1"/>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A23" s="6" t="s">
         <v>44</v>
       </c>
@@ -1962,7 +2020,7 @@
       <c r="G23" s="1"/>
       <c r="H23" s="1"/>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A24" s="6" t="s">
         <v>45</v>
       </c>
@@ -1987,8 +2045,11 @@
       <c r="H24" s="8">
         <v>56</v>
       </c>
-    </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I24" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A25" s="6" t="s">
         <v>47</v>
       </c>
@@ -2013,8 +2074,11 @@
       <c r="H25" s="8">
         <v>58</v>
       </c>
-    </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I25" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A26" s="6" t="s">
         <v>48</v>
       </c>
@@ -2039,8 +2103,11 @@
       <c r="H26" s="8">
         <v>138</v>
       </c>
-    </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I26" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A27" s="6" t="s">
         <v>49</v>
       </c>
@@ -2065,8 +2132,11 @@
       <c r="H27" s="8">
         <v>222</v>
       </c>
-    </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I27" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A28" s="6" t="s">
         <v>50</v>
       </c>
@@ -2091,8 +2161,11 @@
       <c r="H28" s="8">
         <v>325</v>
       </c>
-    </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I28" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A29" s="6" t="s">
         <v>51</v>
       </c>
@@ -2117,8 +2190,11 @@
       <c r="H29" s="8">
         <v>913</v>
       </c>
-    </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I29" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A30" s="6"/>
       <c r="B30" s="1"/>
       <c r="C30" s="5"/>
@@ -2127,8 +2203,9 @@
       <c r="F30" s="1"/>
       <c r="G30" s="1"/>
       <c r="H30" s="1"/>
-    </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I30" s="8"/>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A31" s="6" t="s">
         <v>52</v>
       </c>
@@ -2140,7 +2217,7 @@
       <c r="G31" s="1"/>
       <c r="H31" s="1"/>
     </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A32" s="1" t="s">
         <v>53</v>
       </c>
@@ -2165,8 +2242,11 @@
       <c r="H32" s="8">
         <v>747</v>
       </c>
-    </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I32" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A33" s="1" t="s">
         <v>55</v>
       </c>
@@ -2191,8 +2271,11 @@
       <c r="H33" s="8">
         <v>467</v>
       </c>
-    </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I33" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A34" s="1" t="s">
         <v>57</v>
       </c>
@@ -2217,8 +2300,11 @@
       <c r="H34" s="8">
         <v>7</v>
       </c>
-    </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I34" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A35" s="1" t="s">
         <v>59</v>
       </c>
@@ -2243,8 +2329,11 @@
       <c r="H35" s="8">
         <v>132</v>
       </c>
-    </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I35" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A36" s="1" t="s">
         <v>61</v>
       </c>
@@ -2269,8 +2358,11 @@
       <c r="H36" s="8">
         <v>123</v>
       </c>
-    </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I36" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A37" s="1" t="s">
         <v>63</v>
       </c>
@@ -2295,8 +2387,11 @@
       <c r="H37" s="8">
         <v>41</v>
       </c>
-    </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I37" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A38" s="1" t="s">
         <v>65</v>
       </c>
@@ -2320,6 +2415,9 @@
       </c>
       <c r="H38" s="8">
         <v>12</v>
+      </c>
+      <c r="I38" s="8">
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -14058,15 +14156,15 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B4F8E173-517A-E143-82D0-E59C81DE1A15}">
-  <dimension ref="A1:H29"/>
+  <dimension ref="A1:I29"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I38" sqref="I38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:8" ht="48" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9" ht="48" x14ac:dyDescent="0.2">
       <c r="A1" s="13" t="s">
         <v>133</v>
       </c>
@@ -14091,8 +14189,11 @@
       <c r="H1" s="12" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I1" s="16" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2" s="6" t="s">
         <v>8</v>
       </c>
@@ -14117,8 +14218,11 @@
       <c r="H2" s="8">
         <v>893</v>
       </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I2" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A3" s="6" t="s">
         <v>10</v>
       </c>
@@ -14143,8 +14247,11 @@
       <c r="H3" s="8">
         <v>10641</v>
       </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I3" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A4" s="6" t="s">
         <v>12</v>
       </c>
@@ -14169,8 +14276,11 @@
       <c r="H4" s="8">
         <v>305</v>
       </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I4" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A5" s="6" t="s">
         <v>14</v>
       </c>
@@ -14195,8 +14305,11 @@
       <c r="H5" s="8">
         <v>2484</v>
       </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I5" s="112">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A6" s="6" t="s">
         <v>16</v>
       </c>
@@ -14221,8 +14334,11 @@
       <c r="H6" s="8">
         <v>11172</v>
       </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I6" s="112">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A7" s="6" t="s">
         <v>18</v>
       </c>
@@ -14247,8 +14363,11 @@
       <c r="H7" s="8">
         <v>34854</v>
       </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I7" s="112">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A8" s="6" t="s">
         <v>20</v>
       </c>
@@ -14273,8 +14392,11 @@
       <c r="H8" s="8">
         <v>798</v>
       </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I8" s="112">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A9" s="6" t="s">
         <v>22</v>
       </c>
@@ -14299,8 +14421,11 @@
       <c r="H9" s="8">
         <v>472</v>
       </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I9" s="112">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A10" s="6" t="s">
         <v>24</v>
       </c>
@@ -14325,8 +14450,11 @@
       <c r="H10" s="8">
         <v>482</v>
       </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I10" s="112">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A11" s="6" t="s">
         <v>26</v>
       </c>
@@ -14351,8 +14479,11 @@
       <c r="H11" s="8">
         <v>3609</v>
       </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I11" s="112">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A12" s="6" t="s">
         <v>28</v>
       </c>
@@ -14377,8 +14508,11 @@
       <c r="H12" s="8">
         <v>1434</v>
       </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I12" s="112">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A13" s="6" t="s">
         <v>30</v>
       </c>
@@ -14403,8 +14537,11 @@
       <c r="H13" s="8">
         <v>153</v>
       </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I13" s="112">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A14" s="6" t="s">
         <v>32</v>
       </c>
@@ -14429,8 +14566,11 @@
       <c r="H14" s="8">
         <v>283</v>
       </c>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I14" s="112">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A15" s="6" t="s">
         <v>34</v>
       </c>
@@ -14455,8 +14595,11 @@
       <c r="H15" s="8">
         <v>2202</v>
       </c>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I15" s="112">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A16" s="6" t="s">
         <v>36</v>
       </c>
@@ -14481,8 +14624,11 @@
       <c r="H16" s="8">
         <v>129</v>
       </c>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I16" s="112">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A17" s="6"/>
       <c r="B17" s="1"/>
       <c r="C17" s="5"/>
@@ -14492,7 +14638,7 @@
       <c r="G17" s="1"/>
       <c r="H17" s="1"/>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A18" s="6" t="s">
         <v>38</v>
       </c>
@@ -14517,8 +14663,11 @@
       <c r="H18" s="8">
         <v>61568</v>
       </c>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I18" s="112">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A19" s="6" t="s">
         <v>40</v>
       </c>
@@ -14543,8 +14692,11 @@
       <c r="H19" s="8">
         <v>8270</v>
       </c>
-    </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I19" s="112">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A20" s="6"/>
       <c r="B20" s="1"/>
       <c r="C20" s="7"/>
@@ -14554,7 +14706,7 @@
       <c r="G20" s="8"/>
       <c r="H20" s="8"/>
     </row>
-    <row r="21" spans="1:8" ht="24" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:9" ht="24" x14ac:dyDescent="0.2">
       <c r="A21" s="9" t="s">
         <v>42</v>
       </c>
@@ -14579,8 +14731,11 @@
       <c r="H21" s="11">
         <v>69910</v>
       </c>
-    </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I21" s="112">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A22" s="6"/>
       <c r="B22" s="1"/>
       <c r="C22" s="5"/>
@@ -14590,7 +14745,7 @@
       <c r="G22" s="1"/>
       <c r="H22" s="1"/>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A23" s="6" t="s">
         <v>44</v>
       </c>
@@ -14602,7 +14757,7 @@
       <c r="G23" s="1"/>
       <c r="H23" s="1"/>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A24" s="6" t="s">
         <v>45</v>
       </c>
@@ -14627,8 +14782,11 @@
       <c r="H24" s="8">
         <v>882</v>
       </c>
-    </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I24" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A25" s="6" t="s">
         <v>47</v>
       </c>
@@ -14653,8 +14811,11 @@
       <c r="H25" s="8">
         <v>1054</v>
       </c>
-    </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I25" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A26" s="6" t="s">
         <v>48</v>
       </c>
@@ -14679,8 +14840,11 @@
       <c r="H26" s="8">
         <v>1906</v>
       </c>
-    </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I26" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A27" s="6" t="s">
         <v>49</v>
       </c>
@@ -14705,8 +14869,11 @@
       <c r="H27" s="8">
         <v>6591</v>
       </c>
-    </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I27" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A28" s="6" t="s">
         <v>50</v>
       </c>
@@ -14731,8 +14898,11 @@
       <c r="H28" s="8">
         <v>7959</v>
       </c>
-    </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I28" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A29" s="6" t="s">
         <v>51</v>
       </c>
@@ -14756,6 +14926,9 @@
       </c>
       <c r="H29" s="8">
         <v>51446</v>
+      </c>
+      <c r="I29" s="8">
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -27884,7 +28057,7 @@
   <dimension ref="A1:K39"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="H1" sqref="H1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>